<commit_message>
Listo 1_d pero cambios elementales en las bases del trabajo
</commit_message>
<xml_diff>
--- a/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
+++ b/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Pablo\2024\Bases de Datos Avanzadas\Bases de Datos Temporales\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECC5E09-3CCB-4FE8-A5BE-46080FE2408F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A2B5E3-7547-4D2B-849E-51655AF46CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Docente</t>
   </si>
@@ -233,13 +233,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="I2:Q55"/>
+  <dimension ref="I2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,20 +613,20 @@
     <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="12" t="s">
+    <row r="2" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-    </row>
-    <row r="3" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+    </row>
+    <row r="3" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -655,17 +655,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I5" s="12" t="s">
+    <row r="5" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-    </row>
-    <row r="6" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I6" s="2" t="s">
         <v>1</v>
       </c>
@@ -685,20 +685,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I8" s="12" t="s">
+    <row r="8" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="M8" s="12" t="s">
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="M8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-    </row>
-    <row r="9" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+    </row>
+    <row r="9" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
@@ -721,18 +721,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="12" t="s">
+    <row r="11" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="9:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" spans="9:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="3" t="s">
         <v>2</v>
       </c>
@@ -742,7 +742,7 @@
       <c r="K12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="M12" s="1" t="s">
@@ -755,25 +755,26 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="9:18" x14ac:dyDescent="0.25">
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
     </row>
-    <row r="14" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I14" s="13" t="s">
         <v>24</v>
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-      <c r="N14" s="13" t="s">
+      <c r="M14" s="13"/>
+      <c r="O14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-    </row>
-    <row r="15" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+    </row>
+    <row r="15" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I15" s="2" t="s">
         <v>25</v>
       </c>
@@ -786,16 +787,19 @@
       <c r="L15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="M15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="Q15" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -832,9 +836,9 @@
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="M8:P8"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="O14:R14"/>
     <mergeCell ref="I11:O11"/>
+    <mergeCell ref="I14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1_i hecha, maté tabla Licencia, taché pdf, modifiqué tabla Inasistencia, corregí excel, CREATE e inserts de Docente en 1_a
</commit_message>
<xml_diff>
--- a/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
+++ b/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Pablo\2024\Bases de Datos Avanzadas\Bases de Datos Temporales\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A2B5E3-7547-4D2B-849E-51655AF46CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB46819-2AA5-44A1-B4B9-7C4475922732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Docente</t>
   </si>
@@ -99,15 +99,6 @@
     <t>Ciudad</t>
   </si>
   <si>
-    <t>Licencia</t>
-  </si>
-  <si>
-    <t>idLicencia</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
     <t>Desde</t>
   </si>
   <si>
@@ -120,10 +111,10 @@
     <t>idInasistencia</t>
   </si>
   <si>
-    <t>Justifica</t>
-  </si>
-  <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Justificación</t>
   </si>
 </sst>
 </file>
@@ -586,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="I2:R55"/>
+  <dimension ref="I2:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:M14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +590,7 @@
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
@@ -613,7 +604,7 @@
     <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I2" s="13" t="s">
         <v>0</v>
       </c>
@@ -626,7 +617,7 @@
       <c r="P2" s="13"/>
       <c r="Q2" s="13"/>
     </row>
-    <row r="3" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
@@ -655,7 +646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I5" s="13" t="s">
         <v>8</v>
       </c>
@@ -665,7 +656,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I6" s="2" t="s">
         <v>1</v>
       </c>
@@ -685,7 +676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I8" s="13" t="s">
         <v>18</v>
       </c>
@@ -698,7 +689,7 @@
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
     </row>
-    <row r="9" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
@@ -721,7 +712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I11" s="13" t="s">
         <v>11</v>
       </c>
@@ -732,7 +723,7 @@
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
     </row>
-    <row r="12" spans="9:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="9:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="3" t="s">
         <v>2</v>
       </c>
@@ -740,10 +731,10 @@
         <v>12</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>14</v>
@@ -755,52 +746,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="9:17" x14ac:dyDescent="0.25">
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
     </row>
-    <row r="14" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="O14" s="14" t="s">
+    <row r="14" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="J14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-    </row>
-    <row r="15" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="35" spans="14:16" x14ac:dyDescent="0.25">
@@ -831,14 +800,13 @@
     <row r="54" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="I2:Q2"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="M8:P8"/>
-    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="J14:M14"/>
     <mergeCell ref="I11:O11"/>
-    <mergeCell ref="I14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Transición a sólo tt completada
</commit_message>
<xml_diff>
--- a/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
+++ b/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Pablo\2024\Bases de Datos Avanzadas\Bases de Datos Temporales\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB46819-2AA5-44A1-B4B9-7C4475922732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE3DB8F-09B2-4FD9-AEEA-14C39CDC9F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Docente</t>
   </si>
@@ -97,12 +97,6 @@
   </si>
   <si>
     <t>Ciudad</t>
-  </si>
-  <si>
-    <t>Desde</t>
-  </si>
-  <si>
-    <t>Hasta</t>
   </si>
   <si>
     <t>Inasistencia</t>
@@ -207,28 +201,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -577,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="I2:Q55"/>
+  <dimension ref="I1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,11 +600,13 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
     <col min="20" max="20" width="12.85546875" customWidth="1"/>
@@ -604,186 +617,268 @@
     <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+    </row>
     <row r="2" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="P3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+    </row>
     <row r="5" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
     </row>
     <row r="6" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+    </row>
+    <row r="7" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
     </row>
     <row r="8" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="M8" s="13" t="s">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="5"/>
     </row>
     <row r="9" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="L9" s="5"/>
+      <c r="M9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
     </row>
     <row r="11" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="9:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="11" t="s">
+      <c r="K12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I14" s="5"/>
+      <c r="J14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="12" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I15" s="5"/>
+      <c r="J15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="J14" s="14" t="s">
+      <c r="K15" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="J15" s="2" t="s">
+      <c r="L15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="9:17" x14ac:dyDescent="0.25">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
     </row>
     <row r="35" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="14:16" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="14:16" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P37" s="5"/>
-    </row>
-    <row r="38" spans="14:16" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="14:16" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="14:16" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P37" s="2"/>
+    </row>
+    <row r="38" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -806,7 +901,7 @@
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="M8:P8"/>
     <mergeCell ref="J14:M14"/>
-    <mergeCell ref="I11:O11"/>
+    <mergeCell ref="I11:M11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modifico tabla Inasistencias y acomodo lo necesario para esto
</commit_message>
<xml_diff>
--- a/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
+++ b/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Pablo\2024\Bases de Datos Avanzadas\Bases de Datos Temporales\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE3DB8F-09B2-4FD9-AEEA-14C39CDC9F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA6C719-4711-48F4-A0E3-78941737C497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Docente</t>
   </si>
@@ -108,7 +108,13 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>Justificación</t>
+    <t>Justificacion</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>idJustificacion</t>
   </si>
 </sst>
 </file>
@@ -201,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -209,38 +215,44 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,7 +603,7 @@
   <dimension ref="I1:Q55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +611,12 @@
     <col min="5" max="5" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
@@ -618,254 +629,256 @@
   </cols>
   <sheetData>
     <row r="1" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
     </row>
     <row r="3" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="P3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="3" t="s">
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="5"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="6" t="s">
+      <c r="L9" s="3"/>
+      <c r="M9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="O9" s="7" t="s">
+      <c r="O9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P9" s="7" t="s">
+      <c r="P9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="5"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="9:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="5"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I14" s="5"/>
-      <c r="J14" s="4" t="s">
+      <c r="I14" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="N14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O14" s="12"/>
+      <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I15" s="5"/>
-      <c r="J15" s="6" t="s">
+      <c r="I15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="7" t="s">
+      <c r="J15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="K15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="M15" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
+      <c r="L15" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
     </row>
     <row r="35" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N35" s="1"/>
@@ -895,13 +908,14 @@
     <row r="54" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="I2:Q2"/>
     <mergeCell ref="I5:N5"/>
     <mergeCell ref="I8:K8"/>
     <mergeCell ref="M8:P8"/>
-    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="I14:L14"/>
     <mergeCell ref="I11:M11"/>
+    <mergeCell ref="N14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revisión de cada query, unifico Inserts, actualizo DER
</commit_message>
<xml_diff>
--- a/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
+++ b/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Pablo\2024\Bases de Datos Avanzadas\Bases de Datos Temporales\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA6C719-4711-48F4-A0E3-78941737C497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EFA4AC-890D-416B-B0EA-AB08138EF91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Docente</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Suplente_titular</t>
   </si>
   <si>
-    <t>SalarioBrutoTotal</t>
-  </si>
-  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -115,6 +112,15 @@
   </si>
   <si>
     <t>idJustificacion</t>
+  </si>
+  <si>
+    <t>SalarioBruto</t>
+  </si>
+  <si>
+    <t>ForeignKey</t>
+  </si>
+  <si>
+    <t>PrimaryKey</t>
   </si>
 </sst>
 </file>
@@ -207,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -242,17 +248,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -276,22 +284,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>168287</xdr:rowOff>
+      <xdr:colOff>471657</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2C96437-8749-F2B0-A8EB-FDD740314C5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1AA35D2-61D9-9FF1-DFD7-699063BA3298}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -314,8 +322,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="95250" y="0"/>
-          <a:ext cx="5295900" cy="4749812"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5435863" cy="3653118"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -602,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="I1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,17 +648,17 @@
       <c r="Q1" s="3"/>
     </row>
     <row r="2" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
     <row r="3" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I3" s="4" t="s">
@@ -675,10 +683,10 @@
         <v>7</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="9:17" x14ac:dyDescent="0.25">
@@ -693,14 +701,14 @@
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -722,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
@@ -740,18 +748,18 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
+      <c r="I8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="9:17" x14ac:dyDescent="0.25">
@@ -762,20 +770,20 @@
         <v>9</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" s="5" t="s">
+      <c r="P9" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
@@ -791,13 +799,13 @@
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
@@ -817,7 +825,7 @@
         <v>15</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -836,36 +844,36 @@
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I14" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="N14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="O14" s="12"/>
+      <c r="I14" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="N14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="17"/>
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I15" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="K15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" s="13" t="s">
+      <c r="L15" s="14" t="s">
         <v>28</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="Q15" s="3"/>
     </row>
@@ -879,6 +887,14 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="35" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N35" s="1"/>

</xml_diff>

<commit_message>
Que qué cambié? Qué no cambié. Terminé el TP de Temporales papá, lo demás no importa
</commit_message>
<xml_diff>
--- a/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
+++ b/2024/Bases de Datos Avanzadas/Bases de Datos Temporales/TP/TablasTPTemporales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Pablo\2024\Bases de Datos Avanzadas\Bases de Datos Temporales\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EFA4AC-890D-416B-B0EA-AB08138EF91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A725F7BA-BDBE-436A-85EF-3724922BB42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Docente</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>PrimaryKey</t>
+  </si>
+  <si>
+    <t>Vivienda</t>
+  </si>
+  <si>
+    <t>CUILDocente</t>
+  </si>
+  <si>
+    <t>DNIConviviente</t>
+  </si>
+  <si>
+    <t>idVivienda</t>
   </si>
 </sst>
 </file>
@@ -163,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +185,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -224,42 +248,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -608,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="I1:Q55"/>
+  <dimension ref="H1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,13 +650,15 @@
     <col min="5" max="5" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
     <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" customWidth="1"/>
     <col min="20" max="20" width="12.85546875" customWidth="1"/>
@@ -636,286 +669,504 @@
     <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I2" s="17" t="s">
+    <row r="1" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H1" s="9"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H2" s="9"/>
+      <c r="I2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-    </row>
-    <row r="3" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I3" s="4" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H3" s="9"/>
+      <c r="I3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I5" s="17" t="s">
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H4" s="9"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H5" s="9"/>
+      <c r="I5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I6" s="4" t="s">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+      <c r="I6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="N6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I8" s="17" t="s">
+      <c r="O6" s="10"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H8" s="9"/>
+      <c r="I8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="17" t="s">
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H9" s="9"/>
+      <c r="I9" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="9"/>
+      <c r="O9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H11" s="9"/>
+      <c r="I11" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="4" t="s">
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="8:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="9"/>
+      <c r="I12" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="J12" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="K12" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="L12" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I11" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="9:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I12" s="9" t="s">
+      <c r="M12" s="9"/>
+      <c r="N12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="P12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="Q12" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I14" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="N14" s="17" t="s">
+      <c r="Q13" s="10"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H14" s="9"/>
+      <c r="I14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="14" t="s">
+      <c r="O14" s="7"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H15" s="9"/>
+      <c r="I15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="12" t="s">
+      <c r="O15" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I17" s="16" t="s">
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H17" s="9"/>
+      <c r="I17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="15" t="s">
+      <c r="J17" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-    </row>
-    <row r="36" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+    </row>
+    <row r="18" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+    </row>
+    <row r="20" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+    </row>
+    <row r="21" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+    </row>
+    <row r="22" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="9"/>
+    </row>
+    <row r="23" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="9"/>
+    </row>
+    <row r="24" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="11"/>
+    </row>
+    <row r="25" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+    </row>
+    <row r="26" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+    </row>
+    <row r="27" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+    </row>
+    <row r="29" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="32" spans="8:19" x14ac:dyDescent="0.25">
+      <c r="P32" s="4"/>
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="Q33" s="3"/>
+    </row>
+    <row r="34" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="Q34" s="3"/>
+    </row>
+    <row r="35" spans="16:18" x14ac:dyDescent="0.25">
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+    </row>
+    <row r="36" spans="16:18" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+    </row>
+    <row r="37" spans="16:18" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="14:16" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="14:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="16:18" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="16:18" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="16:18" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="16:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -924,14 +1175,15 @@
     <row r="54" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="I2:Q2"/>
     <mergeCell ref="I5:N5"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="O8:Q8"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="I8:M8"/>
+    <mergeCell ref="N14:O14"/>
     <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I11:M11"/>
-    <mergeCell ref="N14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>